<commit_message>
using data on TC
</commit_message>
<xml_diff>
--- a/Data Files/Constants.xlsx
+++ b/Data Files/Constants.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BD6269-534C-4120-BC7F-424A215C65E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D88622-C987-43AE-B22F-1527DE1F56DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4764" yWindow="2304" windowWidth="11952" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="searchProduct" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>productName</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Happy Ninja</t>
   </si>
   <si>
-    <t>Ninja Silhouette</t>
-  </si>
-  <si>
     <t>Patient Ninja</t>
   </si>
   <si>
@@ -43,7 +40,19 @@
     <t>Ship Your Idea</t>
   </si>
   <si>
-    <t>Woo Album #1</t>
+    <t>Woo Album 1</t>
+  </si>
+  <si>
+    <t>Woo Album 2</t>
+  </si>
+  <si>
+    <t>Woo Album 3</t>
+  </si>
+  <si>
+    <t>Woo Album 4</t>
+  </si>
+  <si>
+    <t>Woo Logo</t>
   </si>
 </sst>
 </file>
@@ -361,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,27 +398,42 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>